<commit_message>
Update Alpha aiJobsOS 0.1
</commit_message>
<xml_diff>
--- a/index.xlsx
+++ b/index.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Il mio Drive\Progetti\ntJobsAI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54222159-BE10-43FE-AB43-C7FE557C6D1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F827A3D-B18D-4078-971E-F3B22712AD5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="103">
   <si>
     <t>NAME</t>
   </si>
@@ -313,6 +313,30 @@
   </si>
   <si>
     <t>Dizionari e funzioni base</t>
+  </si>
+  <si>
+    <t>admin_pytest.cmd</t>
+  </si>
+  <si>
+    <t>Esecuione test</t>
+  </si>
+  <si>
+    <t>ntjobs_billing.csv</t>
+  </si>
+  <si>
+    <t>Biling file di esecuzione jobs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">acJobsOS.py   </t>
+  </si>
+  <si>
+    <t>Classe principale acJobsOS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aiobsJobsJobs.py      </t>
+  </si>
+  <si>
+    <t>SubClasse JobsOS.Jobs</t>
   </si>
 </sst>
 </file>
@@ -712,10 +736,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K1048504"/>
+  <dimension ref="A1:K1048508"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -801,26 +825,29 @@
       </c>
     </row>
     <row r="3" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>56</v>
+      <c r="A3" s="7" t="s">
+        <v>101</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="C3" s="3">
+        <v>102</v>
+      </c>
+      <c r="C3" s="6">
         <v>1</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="I3" s="9">
         <v>46029</v>
@@ -830,61 +857,32 @@
       </c>
     </row>
     <row r="4" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="3">
-        <v>10</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="I4" s="9">
-        <v>46029</v>
-      </c>
-      <c r="J4" s="5" t="s">
-        <v>14</v>
-      </c>
+      <c r="A4" s="7"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="6"/>
+      <c r="I4" s="9"/>
     </row>
     <row r="5" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" s="6">
-        <v>2</v>
+        <v>57</v>
+      </c>
+      <c r="C5" s="3">
+        <v>1</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="I5" s="9">
         <v>46029</v>
@@ -895,49 +893,51 @@
     </row>
     <row r="6" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>61</v>
+        <v>18</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="C6" s="6">
-        <v>1</v>
+        <v>19</v>
+      </c>
+      <c r="C6" s="3">
+        <v>10</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="H6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="I6" s="9"/>
+      <c r="I6" s="9">
+        <v>46029</v>
+      </c>
       <c r="J6" s="5" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>62</v>
+        <v>24</v>
       </c>
       <c r="C7" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>25</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>70</v>
+        <v>22</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>13</v>
@@ -948,23 +948,25 @@
       <c r="H7" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="I7" s="9"/>
+      <c r="I7" s="9">
+        <v>46029</v>
+      </c>
       <c r="J7" s="5" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>54</v>
+        <v>99</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>55</v>
+        <v>100</v>
       </c>
       <c r="C8" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>25</v>
+        <v>2</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>22</v>
@@ -979,7 +981,7 @@
         <v>3</v>
       </c>
       <c r="I8" s="9">
-        <v>46047</v>
+        <v>46059</v>
       </c>
       <c r="J8" s="5" t="s">
         <v>14</v>
@@ -987,16 +989,16 @@
     </row>
     <row r="9" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>81</v>
+        <v>61</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>94</v>
+        <v>62</v>
       </c>
       <c r="C9" s="6">
         <v>1</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>25</v>
+        <v>2</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>22</v>
@@ -1010,28 +1012,26 @@
       <c r="H9" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="I9" s="9">
-        <v>46047</v>
-      </c>
+      <c r="I9" s="9"/>
       <c r="J9" s="5" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>93</v>
+        <v>62</v>
       </c>
       <c r="C10" s="6">
         <v>1</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>25</v>
+        <v>2</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>22</v>
+        <v>70</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>13</v>
@@ -1042,19 +1042,17 @@
       <c r="H10" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="I10" s="9">
-        <v>46047</v>
-      </c>
+      <c r="I10" s="9"/>
       <c r="J10" s="5" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>84</v>
+        <v>54</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>92</v>
+        <v>55</v>
       </c>
       <c r="C11" s="6">
         <v>1</v>
@@ -1083,10 +1081,10 @@
     </row>
     <row r="12" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="C12" s="6">
         <v>1</v>
@@ -1115,10 +1113,10 @@
     </row>
     <row r="13" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="C13" s="6">
         <v>1</v>
@@ -1147,10 +1145,10 @@
     </row>
     <row r="14" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="C14" s="6">
         <v>1</v>
@@ -1179,10 +1177,10 @@
     </row>
     <row r="15" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C15" s="6">
         <v>1</v>
@@ -1211,10 +1209,10 @@
     </row>
     <row r="16" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="C16" s="6">
         <v>1</v>
@@ -1235,36 +1233,39 @@
         <v>3</v>
       </c>
       <c r="I16" s="9">
-        <v>46031</v>
+        <v>46047</v>
       </c>
       <c r="J16" s="5" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="B17" s="14" t="s">
-        <v>59</v>
+      <c r="A17" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>88</v>
       </c>
       <c r="C17" s="6">
         <v>1</v>
       </c>
-      <c r="D17" s="15" t="s">
+      <c r="D17" s="3" t="s">
         <v>25</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="H17" s="3" t="s">
         <v>3</v>
       </c>
       <c r="I17" s="9">
-        <v>46029</v>
+        <v>46047</v>
       </c>
       <c r="J17" s="5" t="s">
         <v>14</v>
@@ -1272,10 +1273,10 @@
     </row>
     <row r="18" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>64</v>
+        <v>86</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>66</v>
+        <v>89</v>
       </c>
       <c r="C18" s="6">
         <v>1</v>
@@ -1284,7 +1285,7 @@
         <v>25</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>70</v>
+        <v>22</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>13</v>
@@ -1293,10 +1294,10 @@
         <v>13</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="I18" s="9">
-        <v>46029</v>
+        <v>46047</v>
       </c>
       <c r="J18" s="5" t="s">
         <v>14</v>
@@ -1304,19 +1305,19 @@
     </row>
     <row r="19" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="C19" s="6">
         <v>1</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>70</v>
+        <v>22</v>
       </c>
       <c r="F19" s="3" t="s">
         <v>13</v>
@@ -1325,36 +1326,33 @@
         <v>13</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="I19" s="9">
-        <v>46029</v>
+        <v>46031</v>
       </c>
       <c r="J19" s="5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="C20" s="3">
-        <v>10</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>3</v>
+    <row r="20" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="C20" s="6">
+        <v>1</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>25</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>75</v>
+        <v>16</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G20" s="4" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="H20" s="3" t="s">
         <v>3</v>
@@ -1366,21 +1364,21 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="C21" s="3">
+        <v>64</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="C21" s="6">
         <v>1</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F21" s="3" t="s">
         <v>13</v>
@@ -1389,7 +1387,7 @@
         <v>13</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="I21" s="9">
         <v>46029</v>
@@ -1398,21 +1396,21 @@
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="C22" s="3">
-        <v>10</v>
+        <v>65</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C22" s="6">
+        <v>1</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F22" s="3" t="s">
         <v>13</v>
@@ -1421,7 +1419,7 @@
         <v>13</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="I22" s="9">
         <v>46029</v>
@@ -1432,7 +1430,7 @@
     </row>
     <row r="23" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>71</v>
@@ -1464,19 +1462,19 @@
     </row>
     <row r="24" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="C24" s="3">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>28</v>
+        <v>75</v>
       </c>
       <c r="F24" s="3" t="s">
         <v>13</v>
@@ -1485,7 +1483,7 @@
         <v>13</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="I24" s="9">
         <v>46029</v>
@@ -1496,10 +1494,10 @@
     </row>
     <row r="25" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="C25" s="3">
         <v>10</v>
@@ -1508,7 +1506,7 @@
         <v>3</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>28</v>
+        <v>75</v>
       </c>
       <c r="F25" s="3" t="s">
         <v>13</v>
@@ -1517,7 +1515,7 @@
         <v>13</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="I25" s="9">
         <v>46029</v>
@@ -1526,8 +1524,168 @@
         <v>14</v>
       </c>
     </row>
-    <row r="1048503" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1048504" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C26" s="3">
+        <v>10</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I26" s="9">
+        <v>46059</v>
+      </c>
+      <c r="J26" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C27" s="3">
+        <v>10</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I27" s="9">
+        <v>46029</v>
+      </c>
+      <c r="J27" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C28" s="3">
+        <v>10</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H28" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I28" s="9">
+        <v>46029</v>
+      </c>
+      <c r="J28" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C29" s="3">
+        <v>10</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H29" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I29" s="9">
+        <v>46029</v>
+      </c>
+      <c r="J29" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="C30" s="6">
+        <v>1</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I30" s="9">
+        <v>46059</v>
+      </c>
+      <c r="J30" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1048507" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1048508" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>